<commit_message>
---Se agregó una nueva tabla a la DB: financiacion ---Se modificó ampliamente la tabla produccion_intelectual para cumplir nuevos requerimientos. ---Ahora hay 8 categorías de producciones intelectuales. ---Los aspirantes tienen una nueva vista resumen donde pueden descargar su hoja de vida y adjuntos. ---Se modificó la vista y controlador de producciones intelectuales.
</commit_message>
<xml_diff>
--- a/SQL/Información_aplicativo_admisiones_posgrados_(respuestas).xlsx
+++ b/SQL/Información_aplicativo_admisiones_posgrados_(respuestas).xlsx
@@ -651,8 +651,8 @@
   <dimension ref="A1:AE1027"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>